<commit_message>
20200203 python boj pdf
</commit_message>
<xml_diff>
--- a/python/pdf_probs.xlsx
+++ b/python/pdf_probs.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15U560\Desktop\2020-1\What_I_Studied\python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\multicampus\Desktop\TIL\What_I_Studied\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB42A0CC-44AE-409B-A762-0BA975F780C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21945" yWindow="4365" windowWidth="21600" windowHeight="11385" xr2:uid="{BFDAF271-6542-4997-8777-84924685DA41}"/>
+    <workbookView xWindow="21945" yWindow="4365" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="5">
   <si>
     <t>문제 번호</t>
   </si>
@@ -89,11 +88,15 @@
     <t>O</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -310,28 +313,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -647,11 +650,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBFACF7E-4048-433C-8331-F03C2C8E7E89}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -663,14 +666,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="E1" s="7" t="s">
+      <c r="B1" s="12"/>
+      <c r="E1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="5"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -698,7 +701,7 @@
       <c r="A4" s="3">
         <v>2635</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="3">
@@ -798,7 +801,9 @@
       <c r="A13" s="3">
         <v>10157</v>
       </c>
-      <c r="B13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="E13" s="3">
         <v>2573</v>
       </c>
@@ -901,75 +906,75 @@
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
+      <c r="A22" s="5">
         <v>2491</v>
       </c>
-      <c r="B22" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="6">
+      <c r="B22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="5">
         <v>15971</v>
       </c>
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="11"/>
-      <c r="E23" s="10">
+      <c r="A23" s="10"/>
+      <c r="B23" s="9"/>
+      <c r="E23" s="8">
         <v>2606</v>
       </c>
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E24" s="10">
+      <c r="E24" s="8">
         <v>2607</v>
       </c>
       <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E25" s="6">
+      <c r="E25" s="5">
         <v>2589</v>
       </c>
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E26" s="10">
+      <c r="E26" s="8">
         <v>2591</v>
       </c>
       <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E27" s="6">
+      <c r="E27" s="5">
         <v>2580</v>
       </c>
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E28" s="10">
+      <c r="E28" s="8">
         <v>1799</v>
       </c>
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E29" s="6">
+      <c r="E29" s="5">
         <v>2505</v>
       </c>
       <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E30" s="10">
+      <c r="E30" s="8">
         <v>2529</v>
       </c>
       <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E31" s="6">
+      <c r="E31" s="5">
         <v>10159</v>
       </c>
       <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E32" s="11"/>
+      <c r="E32" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
20200204 python class wrapup etc.
</commit_message>
<xml_diff>
--- a/python/pdf_probs.xlsx
+++ b/python/pdf_probs.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="6">
   <si>
     <t>문제 번호</t>
   </si>
@@ -82,6 +82,10 @@
       </rPr>
       <t>Ad</t>
     </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -654,7 +658,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -791,7 +795,9 @@
       <c r="A12" s="3">
         <v>2527</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B12" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="E12" s="3">
         <v>1268</v>
       </c>

</xml_diff>

<commit_message>
20200206 python swea course note
</commit_message>
<xml_diff>
--- a/python/pdf_probs.xlsx
+++ b/python/pdf_probs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\multicampus\Desktop\TIL\What_I_Studied\python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15U560\Desktop\2020-1\What_I_Studied\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4070CE7D-3AA4-4C41-A7AE-5C05CE371719}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21945" yWindow="4365" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,14 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -100,7 +93,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -654,11 +647,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
20200207 python boj etc.
</commit_message>
<xml_diff>
--- a/python/pdf_probs.xlsx
+++ b/python/pdf_probs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15U560\Desktop\2020-1\What_I_Studied\python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\multicampus\Desktop\TIL\What_I_Studied\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4070CE7D-3AA4-4C41-A7AE-5C05CE371719}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="7">
   <si>
     <t>문제 번호</t>
   </si>
@@ -89,11 +88,15 @@
     <t>O</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -647,11 +650,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -746,7 +749,9 @@
       <c r="A8" s="3">
         <v>2304</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="E8" s="3">
         <v>2636</v>
       </c>
@@ -768,7 +773,9 @@
       <c r="A10" s="3">
         <v>2578</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="E10" s="3">
         <v>2303</v>
       </c>
@@ -778,7 +785,9 @@
       <c r="A11" s="3">
         <v>2477</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="E11" s="3">
         <v>2302</v>
       </c>

</xml_diff>